<commit_message>
Adding date to df
</commit_message>
<xml_diff>
--- a/account_holdings_index.xlsx
+++ b/account_holdings_index.xlsx
@@ -43,10 +43,10 @@
     <t>USDT</t>
   </si>
   <si>
+    <t>BTC</t>
+  </si>
+  <si>
     <t>ATOM</t>
-  </si>
-  <si>
-    <t>BTC</t>
   </si>
   <si>
     <t>ALGO</t>
@@ -479,16 +479,16 @@
         <v>14</v>
       </c>
       <c r="D3">
-        <v>588.00171574</v>
+        <v>863.0471265</v>
       </c>
       <c r="E3">
-        <v>53.24456156</v>
+        <v>90.62048405</v>
       </c>
       <c r="F3">
-        <v>534.75715418</v>
+        <v>772.42664245</v>
       </c>
       <c r="H3">
-        <v>588</v>
+        <v>863.05</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -502,19 +502,19 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>45.3911</v>
+        <v>0.01540148</v>
       </c>
       <c r="E4">
-        <v>0.2372</v>
+        <v>0.01540148</v>
       </c>
       <c r="F4">
-        <v>45.1539</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>11.8093</v>
+        <v>33509</v>
       </c>
       <c r="H4">
-        <v>536.04</v>
+        <v>516.09</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -528,19 +528,19 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>0.01540148</v>
+        <v>24.0438</v>
       </c>
       <c r="E5">
-        <v>0.01540148</v>
+        <v>0.2372</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>23.8066</v>
       </c>
       <c r="G5">
-        <v>34599.4</v>
+        <v>12.7</v>
       </c>
       <c r="H5">
-        <v>532.88</v>
+        <v>305.36</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -563,7 +563,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.86</v>
+        <v>0.8508</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -589,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>2219.01</v>
+        <v>2211.73</v>
       </c>
       <c r="H7">
         <v>0</v>

</xml_diff>

<commit_message>
Added timestamp to code
</commit_message>
<xml_diff>
--- a/account_holdings_index.xlsx
+++ b/account_holdings_index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>currency</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>dollar_value</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
   <si>
     <t>USDC</t>
@@ -65,6 +68,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -117,9 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -423,6 +432,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,14 +458,14 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="2">
+        <v>44382.89266203704</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>1359.22208948</v>
@@ -469,37 +481,37 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="1">
-        <v>1</v>
+      <c r="A3" s="2">
+        <v>44382.89266203704</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>863.0471265</v>
+        <v>1011.67532122</v>
       </c>
       <c r="E3">
-        <v>90.62048405</v>
+        <v>120.41278248</v>
       </c>
       <c r="F3">
-        <v>772.42664245</v>
+        <v>891.26253874</v>
       </c>
       <c r="H3">
-        <v>863.05</v>
+        <v>1011.68</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="1">
-        <v>2</v>
+      <c r="A4" s="2">
+        <v>44382.89266203704</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>0.01540148</v>
@@ -511,99 +523,99 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>33509</v>
+        <v>34055</v>
       </c>
       <c r="H4">
-        <v>516.09</v>
+        <v>524.5</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="1">
-        <v>3</v>
+      <c r="A5" s="2">
+        <v>44382.89266203704</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>24.0438</v>
+        <v>13.1249</v>
       </c>
       <c r="E5">
         <v>0.2372</v>
       </c>
       <c r="F5">
-        <v>23.8066</v>
+        <v>12.8877</v>
       </c>
       <c r="G5">
-        <v>12.7</v>
+        <v>13.8091</v>
       </c>
       <c r="H5">
-        <v>305.36</v>
+        <v>181.24</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="1">
-        <v>4</v>
+      <c r="A6" s="2">
+        <v>44382.89266203704</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0.8855</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="2">
+        <v>44382.89266203704</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>2231.28</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2">
+        <v>44382.89266203704</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0.8508</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>2211.73</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>0</v>

</xml_diff>

<commit_message>
Attempting to add appending code to account csv
</commit_message>
<xml_diff>
--- a/account_holdings_index.xlsx
+++ b/account_holdings_index.xlsx
@@ -459,7 +459,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2">
-        <v>44382.89266203704</v>
+        <v>44383.5343287037</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2">
-        <v>44382.89266203704</v>
+        <v>44383.5343287037</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -491,21 +491,21 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>1011.67532122</v>
+        <v>896.05924946</v>
       </c>
       <c r="E3">
-        <v>120.41278248</v>
+        <v>123.63124776</v>
       </c>
       <c r="F3">
-        <v>891.26253874</v>
+        <v>772.4280017</v>
       </c>
       <c r="H3">
-        <v>1011.68</v>
+        <v>896.0599999999999</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2">
-        <v>44382.89266203704</v>
+        <v>44383.5343287037</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -523,15 +523,15 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>34055</v>
+        <v>34312.7</v>
       </c>
       <c r="H4">
-        <v>524.5</v>
+        <v>528.47</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2">
-        <v>44382.89266203704</v>
+        <v>44383.5343287037</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -540,24 +540,24 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>13.1249</v>
+        <v>22.0802</v>
       </c>
       <c r="E5">
         <v>0.2372</v>
       </c>
       <c r="F5">
-        <v>12.8877</v>
+        <v>21.843</v>
       </c>
       <c r="G5">
-        <v>13.8091</v>
+        <v>13.3314</v>
       </c>
       <c r="H5">
-        <v>181.24</v>
+        <v>294.36</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2">
-        <v>44382.89266203704</v>
+        <v>44383.5343287037</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -575,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.8855</v>
+        <v>0.9287</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2">
-        <v>44382.89266203704</v>
+        <v>44383.5343287037</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -601,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>2231.28</v>
+        <v>2325.29</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2">
-        <v>44382.89266203704</v>
+        <v>44383.5343287037</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Updates to python functions for getting crypto prices and mining efficiency
This update allows me to append my csv files so that I can have a running history of all prices as often as we run the scripts.
</commit_message>
<xml_diff>
--- a/account_holdings_index.xlsx
+++ b/account_holdings_index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>currency</t>
   </si>
@@ -49,13 +49,16 @@
     <t>BTC</t>
   </si>
   <si>
+    <t>BTC3S</t>
+  </si>
+  <si>
+    <t>BTC3L</t>
+  </si>
+  <si>
     <t>ATOM</t>
   </si>
   <si>
     <t>ALGO</t>
-  </si>
-  <si>
-    <t>BTC3S</t>
   </si>
   <si>
     <t>ETH</t>
@@ -428,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,36 +465,36 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2">
-        <v>44408.88965277778</v>
+        <v>44416.96780092592</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2">
-        <v>1782.94087583</v>
+        <v>1326.50294401</v>
       </c>
       <c r="E2">
-        <v>1782.94087583</v>
+        <v>795.32972885</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>531.17321516</v>
       </c>
       <c r="H2">
-        <v>1782.94</v>
+        <v>1326.5</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2">
-        <v>44408.88965277778</v>
+        <v>44416.96780092592</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>1223.29700881</v>
@@ -508,13 +511,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2">
-        <v>44408.88965277778</v>
+        <v>44416.96780092592</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>0.02448253</v>
@@ -526,96 +529,93 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>41717.8</v>
+        <v>44344.6</v>
       </c>
       <c r="H4">
-        <v>1021.36</v>
+        <v>1085.67</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2">
-        <v>44408.88965277778</v>
+        <v>44416.96780092592</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5">
-        <v>0.2366</v>
+        <v>116.1203</v>
       </c>
       <c r="E5">
-        <v>0.2366</v>
+        <v>1.1076</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>12.8448</v>
+        <v>115.0127</v>
       </c>
       <c r="H5">
-        <v>3.04</v>
+        <v>116.12</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2">
-        <v>44408.88965277778</v>
+        <v>44416.96780092592</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>114.3699</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>3.8651</v>
       </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0.8486</v>
+        <v>110.5048</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>114.37</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2">
-        <v>44408.88965277778</v>
+        <v>44416.96780092592</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.2366</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.2366</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
+      <c r="G7">
+        <v>13.402</v>
+      </c>
       <c r="H7">
-        <v>0</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2">
-        <v>44408.88965277778</v>
+        <v>44416.96780092592</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -627,7 +627,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>2521.49</v>
+        <v>0.8378</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -635,24 +635,50 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2">
-        <v>44408.88965277778</v>
+        <v>44416.96780092592</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>3054.33</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2">
+        <v>44416.96780092592</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="H9">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>0</v>
       </c>
     </row>

</xml_diff>